<commit_message>
for larger sequence data
</commit_message>
<xml_diff>
--- a/Swadha/lncRNA_data.xlsx
+++ b/Swadha/lncRNA_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,11 @@
           <t>sequence</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>seq_length</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -459,6 +464,9 @@
           <t>GUGAAAUGCAAAUGAGUUUUUUGAGUUUUUGUUGACACCUCUAACUGCAGGAUGGAAGCGGCACAAAUUGUUCUGAUCAGGGAGCAAUAACAUGCAACGAUCCCCAGGGCUCCCAGGCAGGCGGAGGGGGCACCCAGUCUCAGCAGCCCGCGAUCUGCUUGGCCCCUGCGAGCUGCAUGCCUCACAUUUCCCCAGCUCCAGCCUCCUUUCAAAGGCCCUUUAUUAAACCACCAACUAUUUGCUGUCGAGACAUUUAGGAUGAAAUCAUUGUGUUAAACAAAUAAACGCAGCUUCGUCCAGAUUUCUGCUCUGGGAGCAGAGUAAGAAAAUAAUUUCUGUCUGCUCGCCACAAAAGCGGCUGGAAAGGUCCAAAGAAAAAUAUUAUUUUUACUCCAUUGUGUGAAAUAUUGUCCUGGAGGAUCUGACGGGCUGAGCGUUUGAAGAGUUUGUGCUGGCAGGUUUCAAGGGUCCCCUGGGUCGGCCCCCUGGGAUUGUUUUCUGCAUUAAUAAACUGAGCAUGAUGUGUGUUAAAAAAAAAAAAAAAAAAAAAAAAAAAAA</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>558</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -474,6 +482,9 @@
           <t>GAAGCCCGGGCCAGCCCCAGCGCCCAGCUGGAUCCCGGAAUAACCGGUGAAGACGGCUCCCCGGAAUCCCCGCCCCUAGCGGGCUCUCCCGGACCCCCGGCCCGCGCUAGUCUUUGCCAGGAUCCCGCGCAAAGGAUCAAGUCCCAGCUUCCCUUUCCCCACCGAGAGUCUCCAGCGCCAACCGCGGGCCGUCGGGCGGGUCCCUGACCCGCAGUUACUCAGCUACCUCUCUGGUGGAGGAGGUGUCAGCGACUUGAGAAUGAGUGCGCCAAAGAAGACAGAGCCACGCCUGAGCCUCCUUCAACAAAGCCUGCACUUCCUGUUCUCUUCUCAAGCGUGCUGUCAGCAGAUCUUGACUGAAACCUCUGUGCCCUACCCUGUCCUUGGCACCAGACGCAGGGGAAAGGAUCAGGCCCAGUCCCUCCUCUGACUGACAGUGCUAAACCAGCUACCUGUUCUGAGCAAGGCCCCUGAAGACUGGGAACACGAAUUUGCCCAACAGCUGCCUGGCUUAAGGGUUAGGCCGUUGAUAUAAAAAUACAUGGCUAAUGUAACCUA</t>
         </is>
       </c>
+      <c r="D3" t="n">
+        <v>558</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -489,6 +500,9 @@
           <t>CUCCCCUUCACCAGCUCCGCGGAAACCAUAGCAACGGGCAGCCGGAAGAUGCGGCCAUUCCUCUCCCUUUUGUCCAUUGCAUUUCAGCAGCGCCCGCGCACAUGGACGCUCCAAUUACAGCUCUAGAGGCUAGAAAUUGGCAGUCAGGAUGUGUGUAAGGCCACGCUCCCUCUGAAGACUCCAGGGGAGGAUCUUUCCUUGCCUCCUCCAGCUUCUGGUGGCUGCCAGCAUCCUUGGCAUUCCUUGGCCUGUGGACACAUCACUCUCAUCUCUGCCCAUGGUCACAACCCCAAGCUCCAGAAUACAGACCAGCAGGCGAGGAGACAAGGAGGCAAGCAGAUGGAUGGUGGAACAAAGUGGCAGAGAAAGAGAGAAGAGGAGAGAUGUCUGGACGCCAAGAGGAGUCUGGCUGGGGCCAGUCAGAGAAGAGUCCAGCGGCUGGGCAGCCCGACUCCAGGGGAAGAUCACCUUCCCACUCCAUCCCCCUUCACGCUCCCCAUCCAUCUCACUAAGAGCCAUCUCUACCACUCAAUAAAACCUUGCAUUCAUCCUUCAAA</t>
         </is>
       </c>
+      <c r="D4" t="n">
+        <v>557</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -504,6 +518,9 @@
           <t>AGACUCCUGCAAACAGCAGCUGGCUUAGUGGAGGCUGCCAGACUUCGGGGAUUCUGAGAUCUCUCAGCGAAGAUGCUGAUACAACUUCUGACACUGUUGGUGAUGAGUGGUGCAUAACAGCCGUUUCAGCUCUGAGGCUAUCAAAUAGUGAAAGAGAAUCUUCUACAUACAAAUCCCAGGACACCAGAACAGCUCUUAACAGCCCUCACUUUCCUGAGUAAGCUGAAGGUGGCUAACUAAAAGGCCUGAGAGAAAUUACUGCCUAAACAAUGAAGGAAGGAGAAAACCCCCAAGGAAGACAAUGUAAAGAUUAAGUAACAAGGUUUCAAUUUGAUACAAUGUGGGGAAUUUCAGUUUAAUUCUAAUUUAUACUAAUUUCUCAUAAUUGUCUUGAUCCUUUACGUAGAGAUCGGUUUGGAUAAAGGAAUCAUAGCUAUGAGAAGGCAGUUAGUUACUCAGUGAAUCCAAAUGGCAAAUUCUCUGAUGAGAAAGGGGAUGUCCUCAGGGAGGUCUAAUCAUAUGUUUUCUUAAACCAAACUCUUUUCCUUUUCAUUAG</t>
         </is>
       </c>
+      <c r="D5" t="n">
+        <v>556</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -518,6 +535,189 @@
         <is>
           <t>AAGAAGUGCCUUUCACCUCUCAUCAUGAUUCUGUGGCCUCCCCAGCCAUGUGGAACUUUUUUCUCUUGCUGCUACCAUGUAAGAAGUGCCUUUCACCUCGUGCCAUGAUUAUGAGACUUCCCCAGCCAUGUGGAACUGUUAAGUCCAAUUAAACAUCUUUUUCUUCUUAGUCCCAGGUUGUUCUCAUUCGUGGCUGGAUCACACCAGCAAGAAGGAUUUUAAAGGACAACUCCUUGGGGCCGUCCAACACUGAAACCGCCUGACCGCUGCUGUCUUUGUGCUUGCAGAAAAUCACGGUGGGCACAAAAUUUUGGACACGAUUUCGAGAGCGUGAGAGCUACUGUUCACGAAUCCAGGGCCAGCCUCGUGUCUGUCUUCCUUUAAAGCACCUGGCUUGGUACCUAAAAUGUUCCUUUUUUUUUUUUUUUUGAAAUUCAAUAACUUCAGAACAGGCGUUGAUGUAGACAGAUCUCCAUCUUUUUGGUUUUUUGAGUGAGUUUUUGCUCUGUAGGCUGAAUUCUUUGGAAUUUAGUUCUGAAAUCACAAAAAAAAAAA</t>
         </is>
+      </c>
+      <c r="D6" t="n">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>URS000075E21A</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>GAACUCCUUACCCCAGCUGCCUGGCUGCCCUCAGCUUCCCAAAGCUCAAAUAAGAGGGGCCGGCGGCGCGGGGAAGAGGAGGAGCCAGGAGGCUCGGCCGCUCCAUUCACUCAGCAGCCCAAGCCCGGCCAGGCAGCGCGCGCUGCUCCUUGGGGGCGCCCUCGCAGCUGGGGUGAGGGCGGGUCCGAGGGAGCGUCCCUCUCGGAGACACCCUCCUCUUCAACCCAACACGCGCUCUCAGCUGGCCGGUGUGGCACAACCCUCCCCCCACCUCCCCUUCUUGGCCUUCGCCAGUGUGGGAGCCUCGUCUCACUGGAGAGUCCGUUCAGAAUCCUUGUGGGGGCGGGGAGGGGAAGAGCACCGGUGCGAACCCCGGGGUGCCCCCUCGCCCGACUUGGACUUCUCCGACUAAAGAGGUGGGAGGAGUUCCCUGCAGCCUGCGGGGCCAAGAAGAAAGUGCUAAGCUGAGGAGCCGCAGUCGGAGGACCCCAGGGACCCGACAGGAAGUCUCCGUACGACCCCAACGGAUCCACAUGCCCGGAAGCCCAGGCGACACUAAGCCAGCGCUGGGGAACUGACGUACUCCUGCAGUCGCAGGGCGCUCCAUGCCUCUCUGUCCUCUUCUUUGUUGUGGGUAACGUUCUCUGCGGGAGACCUGAGGUUUUCCAAGGGGGACAUGCCAGCUACACUGGCCUUGGCGCCCUGAGCUAAGCACCAGGACUCACAGCCUAGCACGAAGGCAGGUAGCACCUUCACCCGCCGCGGACGAUAGGCGCUCUCCUGUACCUCCUUUAGCUCGCGAGGCCCGCCCUUCGCGAGGUCCCAGAGAAAAGCAGGCUGUGGAAAACUGGGCGCCCCCUUCUUUCACCCACCUUCUUACCCCUGUCAGCGCCGAGAUCUGUAGCAGAGGUUCCUGGUCUGAACCACCGAUUGGCAAAGAAAGCUGCAGAUUAAACUUCUCGUUUUACAGAGAAGGAAACUGAGGCCCAGACAGCCGAAGGAGAGGCAGUCUAUGGAGCGCAGCGGUAAAGAGCAAGGGGUUGGUGGCCCCAGAAUGGAACCUCAGCUCUGCCAG</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>URS0000CCE02F</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CAUCAGACACGAAGGAGAGGCCAACAGAUGAGGGAAGCCAUUUUUCUGCAAUGGAAUUAAAUGGCCAAGCCCAAGGACUCACAGUUGGAAGACUGGAGAAGACUUUUUAAAAAGAUCUGGAUUUUUCCUUAUGACUUGGAAUCCAUCUUUGUCUUGUAUAACUAGGUCAUAGCACACCAUUCAUGUCAGCAGUUAACAGUUUUGAAUUCCAAAAAAACCUAAAGCAGUAAACAGUCCUCAGCGAAGCCGCCUUUUUGCCUACCCAACCCUGGAAAGUUUGCAGAAGUGGAAGGAGCAGAACGUGAGGGUGUAACUUACAAAAAGCUUGAUCUUCUAGACUCCAUGGCACCGGGCUGAGCGGGUUCUGGGCCGGAGAAGGGGCGACGUUCGGGCACCCCCCGAAUGGACAAUCUUUCCUUCUGUCAACGGCAGGGGCAGGCCUAGUUUGACUCUGACAGUCCUCCCACUAAGGAAUUCCUGGUGACUGGAAGGGGGAGUGACUCAGGCCCUCAACCUCUAGCAGAGUGCCUUGGCUCCCUCCUGUCGUCCUGGGGAACCUCGGCCCCAGCCCUGCCUCCCCAGCCAGUCACAGCUCCUCCCUGGUCACCCUGAGGGAGCUCAGGGCCCGGCUGGUAGCUGGGUUGCUCUGCUUCUGUCCCCCACUCCUGUGGAGCCUGGCAGGCAACUCCAUGAUCUGACCCCGGUUACCUUGACAGCCCUGCCUGGCCUCCCCUCUCAUGGCCCAGCCACCCCAGAACCUGAAGAGGUUUUCUAGCUGCCGUGCAUUUGCCAGGCUGGGUUACCCACCCUACUUUCCCUGCCUGCCCUCCAGUGCUGCCAGGCCUAGUGUGCCAGCCAGCGCUCAGCCUUCAGUAAAGGGUUCCCCUGCUUCCAACCUCCAUUGCACUGCUUCCCCUAAGACUGUGACCUCCUGGAAGGCUGGAGCACAACUGCCUCUCAAUAAACGUGUUGCAAAAAAGGAAAAAAAAAAAAAAAAAA</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>URS00026A1FD4</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CCUUUCCUGCUUCCUCACCCGCUGUAGCAAGCAGGUGUGGAGUCGAGUCGGAGGCAGGCGCUGGCUGCGUGGACCCCCGGGUGGGAUUCCACCCGCGACAAGGCACCCAGGCCCUUUGGGCGGGGCUCCCCUGGGGUCCGCGUCCCCGCCGCCUCCCCCGGGCCUCUGCUGGGCUGGCUGGAGGCAGGAGGCCCCGGGCCAGCAUCCUGAGCCCCACCUGCAGGCCCUGGGCGCUUUCCUCCUGGCAGCUGUGCCCCCACCCGACCGGACCGCUCCCUGCAACCAGAGAGCCCUCACACCAGCAACACCCCCCAGCCUGCUCCCUCCUCGUGUGCGCGAAACUCAUGGCACUGGCUUGACGGCUUUCUCUGAAACCCUCUGAUUCCGCCUGGCCCAUCCACACUGUCCCUUCCCGGCCAGGGCUCAUCUCCUAUGCCUGGACCAAACAGCGUAGUCUCCAGUCUCCCUGAUCUCCCCACACGUGGCCCCACCCAUCCUCUGAAGCAGCCCCAGGAGGCAGCAGUGACUUCACACUUCUAGUGCCCGGCCCUCCCGGCCCUCCUCUCUGGGCUUGCUUGCCAGGGUCCUCCCAACCUGACUGCUGCCUCCCACCUCCUCUCCGCCCCUGGAGCUCUCCAGCCGCAGCCGCGGGGCCUGCUUGGGAUUCUCCUCUGCUGGCAUCAUCCCUGCCUGCCUCAGCCUUCCCAGGCCCAAUCCUGCCCGAUCUCACCUCUUCCCGCCCAGCCACCUGGUCGGGUCCCGACCAGCAUCUGCCUUCAAACCUGGAGUCCUUCCCUGAGUGCUUGCGGUGCACUGUGAGGAAGGAAAUCAAUGUAAAGGAUUAUGACCCACAUUUUUUAAAAAUAAAAAGAUUAAGGAGAACAGCA</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>URS000075E59E</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>UUGAAGAGAUGAGUGCGGGGCUCAUCUAUCCCUGGAAUUGUCUUUCCCACAAUCCCUGACACAGAAUAUGAGCCAUACAGGAAUUCUGAAGAAAUGGGUCUCUUGCCACCUCCCAGUAAAAGAUUAUUUUUUAAAAAAAAAAGGCUCUGCUUUGACCUGAAGUAUUUUAUCUAUCCUCAGUCUCAGGACACUGUUGAUGGAAUUAAGGCCAAGCACAUCUGCAAAAAAGACAUUGCUGGAGGAGGUGCAAAGAGCUGGAAACCAAGUCUCCAGUCCUGGGAAAAGCAGUGGUAUGGAAAAGCAAUGGAAAGAGCAUUUUGAAAAUGCCAUUCCACUGUUUUCUGGCCUUUAUGAUUUCUGCUGAGAAAUCCACUGUUAGUCUGAUGGGGUCUCCUUCAUAGCACCAAUGACCUGAAGAGCCUUGUUGAAGGAAGACUCCAUCUGAUGACUCAGAGCAAGUAUUUUUUAGUGUGUUAUUGUUAUUAGCAGAAAGAGGGCCAUAAAAUACAUGGGGCAAGCUGAAUAUAUCUUAGGCAAAAGAAGAAAAUAUUCAAAUUCUUAUGUUAUUUUAUCUAAUUAUUUUAUCUCUUUUUGUGUGUGACUUAUAAUGUGUGUAUUGUAUUAAUAAAAGUAUAUAAACAUGUAGUUUACAAAAAAAAAAAAAAA</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>URS000075A563</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>GAGAAGGGAGGAGUUAUUCAGGCCUCCGCCAGCUUCUAGGCCCUGGGGAUGGUCUUUCACCUCCCUCUUUCUGAUCUCUUUUUCAUGCUCCUCCUUGCUCCAAAGAAAAGCCGGAUGGCAAAAGAGCCCAGAACCUAUUGGAACUGACAAAAUCAAGUCACGGCGCCUACAAAGAUGAGGGGCAGAUUCUGGCUGCCUUUUAAUUUCGUCCUUCACCUGAUAUCUGUGCCAGAGAAUGAUAAAAAUCAUAAUAAAGGAAAUAAUGGAAGAGGAGACUUAUGUUACUGGGGACAUCUAACAUAAUUAUUUUCCUGAUUCAGUGGCAUGGUUCAGUCUUCCAGGAGUUCUGCUACAGAGAAGAGAGUAACCCCCAUCCAUCAUGGCCAAAGCACCCAGUCAGGCUCCGCUCUGGAUCCAGCCCGACAAAUGCAACCCUUGAAUAGGGUUUGUGCAAGCAAACUGGAUGACGACCGAAGAAACCCUGUCGCUUCUGAGAAGACACCCAAUCCAAGAAUGUGAGUUCUGGAAAUGUCAUUAAAUGUCAGUUAUAUACAUGCAAAAAAAAAAAAAAAAA</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>URS0000193C7E</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>GGCCGGGCGCGGUGGCUCACGCCUGUAAUCCCAGCUCUCAGGGAGGCUAAGAGGCGGGAGGAUAGCUUGAGCCCAGGAGUUCGAGACCUGCCUGGGCAAUAUAGCGAGACCCCGUUCUCCAGAAAAAGGAAAAAAAAAAACAAAAGACAAAAAAAAAAUAAGCGUAACUUCCCUCAAAGCAACAACCCCCCCCCCCCUUU</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>URS000075B07A</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>AGCGGGCUGCAGGGCUGCGGGCGCUUGGUUCGGCCUGGCCCGGCCGGCGGCUCCUAACACCGGGCGGGCGGCUGCGGCGGCACUUCCGGGUUGGCCUUCUCCAUGUUGGUCUCGGGAACGUGAAGGGGCGGGGCCUCGAGGUCAGGGGUCAGCACCUCCCUGGUUGCCGUGGCGACUGGAGGCGCGCGACGCGGGCGCAAUGGCGGGGACCCGGGGCUUGAUGCUGCUUGGGCCUGGCCCAGUGGCGGGUCCUAGGGACGUGGGUACCUGCAGAGGCCGGCAGAUGGAGAUUCAGAAACAUAAGGACAACAAGAAACUUCCCCAAGGUAUCAUUAUAGUCUUUAGACUUCAGACACACACCACACCUCAAAUAUAUACACAACUGAAAGGAAAAUUAAGGAAGUUUUUCAAAGAACCCUAUUCCGAGUAAGAAGUGUGUUGCAUGAAUUUCUAAGAGCCAGAAAAUGCAUGACACAGGAGAAGAUGUACCCUCAUCUGUUCAGUGAGAGAUGUGCAAAUCAACAUCAACACAGAACUGCUGAAGAAAAAAAAUAUGUCUCUGAAAAGCAACUUAUUCACUGGAGAUGUGAGGAGCCAUCCGCACAUCACAAUUCUAUAGACAUCAAACGCAUGAAGCAUUUCGGAUCUGCUUUAAGACUGAGGCAGACUUUCCAUCUGGACACAGCCGACCAUCCAUGUGUCAUUACAAUGAAUCCAGCACUUCCCUGGAAGCUGGAAGGGUCAAAUUCAACUUCAACUCUGCCACUUCCUGCUUAACUUGCUGUUUAACCUUGGGCAAGCUGCCAUCCCACACGAGGCCGAAGGUGUCGGUUUUUAAAAUACAGAAAUUUGGUUCCAUGAGGGAUUAUCAAUAUACUGCUGGUGGGCCAAAUUCCAUCUGCUACUUGCCUUUGUAAAUAAAGUUUUAUUGAAACACAAACAUGCCCAUUAGUUUACUCUUGUCUGUGACUACAAGGGCAAAGUUGAAUAGUUGUUACAGAGACCAUCAGGCUCACAAAGCCUAGGUUAUUUACUAUCUGCCCAUUUACAGAGUAAGUUUGCCAGCCCUGGACUGGAUAAUUUUUUGAGUUCUUUCUAAUUCUAGAAUUCUUUAUAUAUUUUAUGAAACCCCUAAUGUUUAUAUAUUAAUUAUUUCAAUACCCGUGUCUUUACUGAGUCCCUCCUAUGAAGCAUACAUCAAGACAUAUGUGUGAUACAUUAACUAAACUUUUAACAGUAUCUUAAAUAGGAUUUCAAUGACUAACAGCUCUUGGAAAUAUCCAAGGUAACAUUUGGGGGCAAAUGUCUUAUGAUUUGAUUAUCAUUGGUAAAUAGAGCAUAUCUUUUUUUCCACUAACAAUGUUUAAGAAGUUAAAAAAAAAUCAAGAAAACCCCGUAUGGCACUAGAGACUUAUUGCAUUAAGACAUCAUCUUAACAGAUUGUUUAGUUUUGGUAAUAUAAUUUGACAUCUAAACAUAAGCUGAGAGGGAUCUCCCUCAAAACCUUUGAUAAUAUGAUUCAUUGUCAAAUGUUUGUUUUGCCUAUCUGGCACUCAUUAAUUAAUUCUUUUUAAUAUAGCUUGGAUUUACUGAUUUUGAAAAAGAGAAUUAUUCUUAUUGAUGUUGCUAAAAUAUCCAGGUGGCUUGAAUUUCACCAACUAGAUAGUUUAAUCUAGCACAUUUGUGUAGCCCUAAUCAAAUCUUUACUAACAGAUGUGAGAAGCCCAGUACUGGAGCUAAUGUUUGUGUCUCAAUGAUAAUUAAAUUAGCUUAAUAAGGAAAAUAAAUGAACAAUAAUCACCAAAAUUUUUCCCUAAACCUGUGUUAUAGUCUUAAAAACAUUUUUUCCCCUAUGGAGGCUUUUGGUAAUAAAACACAAAUUGAGGGAUUUUAAUUAAAAGAAAUUUUUUUUUCAAGAACUGGUCAUGUACUAAAUUGCUUAUAAUCAAAUAAUCAAGUAGCAUUUCUUUUAUUAUAAGAGCAAAACCUAUAAUUAAGCCAAAAUUCAAAUUUGUUUUUAAAGGUUGAAUAAUCUUUUGUUUUGGCCAAUAGUAUGUGGAUUUUUUUUUUAAGUAUUAUCUCUUUGUAGUAUUUUCUAAUGGAUAGGAAAUGCCUUUCUCAGGUUGAAUGAUUAUUUCCACAUAGAAUUAGUUCCUGCUUACAACAGUGCUCCACUAAUGUAAUGGCUCGGUGAAUUGGCUUUAUAAUUCAUUAAUCAUAGCUCACAUUGAGCUUUUGGCUCCAGGUGACAGUGCCCACCACAGGCCAAAUAACUUCUCAUUUAAAGGCAAUUUGUACAAAUAGGGAAGGUGAGAAUUCUCACAGUCCCAGAGGGAUUGAAGAGUUUUAAAAAACCAAGAUAAGGCAUUUUAUGGAAGACAGGUUGAUGGAAGAAAAGUGGCCAUUGGAGGAUGAGGCAGAUGGCUUUCCAGGGAGGCCCUGGAGCUGCCACCAUGGGGAAGGCCAUGUUGCAGCUGCUGAUCAGAGCACAUUGGACGGUGUUUCCGUGUGAACAUGAAGACAAUGCUGCCUCUGUUUCUGUGACGCUGUGCUCUGAUCUUGCUGGAGGCGAAGUGGUGUCAGCUGUGCUUACAGGACAGUCAGUGGUGGUAGAAAAGAGGCCAGUGUGACCUGUGAAGGACUGGGCCCCUCUCACUCAACCUGAGUGCCUGCAGUUGUGGCCACCUUUAUUUGUGUAUUCUACUGUAUUUAUUUAUUUGCCUGGCUAAUUAGCUCUGUGCCACAUUCCUAAGCUAGAUGUGUCCCUUCAUGUAAGUGAGAGGGAGACAGAAAGAAAGACUGAGGUGGGGGGUAGGAGAAAGAGAGGAAAGCAAGCAAGAAGAAAGAGAAAGAGAGAAGAAGAAAGGAAGAGGAAAGAAAGAGAGAAAGAGAAAGAGAAGGAAGGAAGGAGAAAGAGAAGGAAAGAAGGAGCCUUCUAAUUUUAUUUCAUUUCUCCAAUAAAUGUUCCUAUAUUAAGACUUUAGACAAAGAUUAGAAAUAUGAUUUGACAGAAAGUGUAUGGAUGUGUUGUUCUAUUGCAUUGUAAGUAAAGUAUCCAUGGCAAUAUACAAAUAAUACAGCUCCUACCCCUAUUCUCUGUUGUUACUUUCAUGUGUUGUCUUAACUUUUUAAAUUUCAAGAUAAUAUUGCGCUUAUUUAUUUUUCCAUGAGGAGGCCUAGGAUUUAGCUUGAUUAGAAAAGCUGUGGAAAAUGAAUGUGCUAAUUACUUUAAAUCAAAUUGAAAAUAAAUUUUAUCCUGUUUCAUGCAAAACAAAAAAAAAAAA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3284</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>URS000075AA30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>AAACAGUUGCUGUGGGGAUUGAAUGACUAGUGCAUGUGAAGCUGCCAGUGUGGUGCCUGCCUCGGGGUUCAUCAAAAACAGGAAGUCAAAGGUCUGAAUACUCUUCCUGUGAAUCAACAGAGAAAGCUUUCUCAUCUGAGCCCAUGAAUACGCAGCCUAGGGCCACUGACUUGUAAGAAUGGAGAGUUGCAAGCUGGACCCUGGGGUAUCAGACAGGCAGAAUCCCUUGCAGCUAGAGUCAUGGAAGCGAAGAAGUUUCCACAAUUAGAUGUGCCUAUGCAAGAUUUGAAAAGAGGAAAUGUGACAAAAGGGCAGAGUUCUGCAGCUUUGACUACUUUUGCUGGCAUGCAAGGUCUUGAAGAUGCUGUGCUUUCCUGCAGCCAAAUUCUACUGUAUAGCCACAAGCUUCAUGAAAACCUUUGGAGUCAUUUUCUUUGGAGCGGGAGUUGGGAUGGUUUGCUGCAGACACCCAGAUGUUUGAUGCUAUGUCCUUUUAUCUUCACCUGCAUGAGGCCGCUUGAUAUUGAUCUCACUGCAGUCCUCACUACAUAGCUCAUUGGAGUCCACACCAUGGCUUCGUACGAGUGUGCACAUGCAGUCAAAGGCACCCUUAAUGCCUGCUGCUCUGCGUCCUUCGAUGUCUCCUGCUCAGCAGUCCAGCUAUUACAAGAGGCACAGAGCUGAGCAUAUUGCUUCAGACCCAGAAGAAUCUCCUCCAUCCCAAUUGGGUACAAUUGUGAAGGAAAUGUGUUGGAGGAAGUCACCUUCUGUGAGCUGCUUAUCCAUCAAGUUGCACUCUGUGUGGGUGUGUAUCCUUCCUAUCUUGGCUGUCUUAGGUCUCCAUAUCCUAGGCAGUAGCCGGGUCAGUAUUCCUUACCAUGCACAUUUGGGCAAUAGAGGUACUGGACAAUAUAGGUAAAUUCACAACCAAUUCUUUCCCUGCAUUUUCUCCAAAUCUGUGGACCAAAUCCUACUUACCCAUGGCCCUACAAAGUUGUCUUUCCUAUCAACACUAACACACCACACCUUGUUUCUCCUAACCUUCCCAGAAUUCCUUGAAGGCUUUCUGAUAUUUGAGGCUUGACAAAAUUUAUUCAUGCAUUGAUUAAGCAGCUAGGAUUUAUUAACCACUGUGAAACAGAAAUUUUGCCAGGCAAUGAAGAUAUUUAGUUGAGUAAGACAGUGCUUCUGUAUUCAAGAAGUCUACCUGUGACCUAUUUUAACUGUAUGUUUCCCUGAAUUUGGGGCAUUCGAAUGGUAUGUACUAAAUGUCUUAUUGGAUGGUUCAUCCUGGAGGAGCGGCUAAUGGAGGCUGGAGUCAAGCUAGGUGUCUGGGCUCAUGUCUACCUUCUUCUGAGUAUCAGAGGGCAGACUCUGAUGUUCUCAGAGAUAGAUGUUCUCAUAGUCUUCGGCUGGAGGAAAUGCCCUUGUUCAUGCCAUCUGUUGACCUGUAGCUACCAUGUAGACCUCUCUGAGGGCCUGUGGCUCAUCAGGAGAUCCGAUGGACACCUGAAUCUCAGAAAAACUGACCUAUGGCACUGUUGUGAUGCACAGGUAUAGGCACAUCUCAAAACAUACCCGUAAAUGUCCCAAGUUUGAAUAUUUUCAAAAUUAUAAGCUUGUAUAUAGCUUAUAUAUUUGCAUUGUAAUCCAUUUGUACAGUACCUAAUUCAAUGCGAGCAAUUACUAAUUUGGAAAUUGUACUGAUAUAAAUAAUUCCUCUCUUUAUUGCAUGUAACACUGUGUCAGUGAUAUAAAAGCUAUGUGUGUAUAUAUAUACAUAUAUAUAAUAUACAGAUGUAUUGAAAUAACUUUUCUAUUUGUAAACAUAAUGGAAUUACUGUAGAAUAUCACCCUCAAGGGAAGGAAGAAAUACAUGUGAGCACUUUCAGGGUAGUUUGCCUGCAUCUGAGCAGUUGUAGAUACUUUGGUGGUAUAACUGGUGAUGAAGAAGAAGGAGGGAAGUUGCAGAGGAAAGAAGCUUGGAGAUGUUUGGGAUAGCUUUUUUAAUUUUCACUGGAGUCGAUUGUGCUAGGGCUUGGUUUUGAGGAUCUGUGGGUAAAUGCUGAGAGGGGUGGGUGCAGUUGCCUAGGCACAAAUAUCUGAAUAGAGCAGAUAUGGAUGAGUGGUUCAGGGGAGGAAAUAUUAUCUGCCUUCUUUUCAUUCUGCUUCAUGCUAGGCAGGGCAAUGAUGAUUGGUUUUCAUUCAGCUUGUGCUCCAAGAGUACCUCAGAAAAUGGGGAGCCAUUUUUCCCCAGUUUUGGUUUUUAGAGGUUUAUAUCCCCAACUGGCUAUGGUUGGCUGGCAGCCUUUAGCUUCAGUGUAGCCACACAUGAUUUCACGUCGUCUGUACAUUCUUCGGCAGGAACCUGCUCCUUUUACUUCCAGUGGACACAGAGCACUUCAGCUAUGGGCAUCCAUAACUACUUCCUCCUGGAUCUGAGGCUUUCUUGGCUCUGAGAGCUUCCUGGGUUUGCUGACCUCACCCCUGUGAGGAGGAGGAUUGGCCCGGCUGCUGAAAACAUACGUGUAAUUGAAGGAAUUCUAUUAAG</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>2551</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>URS000075C848</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>GUGCUUGACUGGAGGAGGGCUGGCAGCAGAAGUGCAGCUGACCGGGUUGCGUUUUCGUACGGCUGACUAAAGCGGAUACCGGUGGCGACUCAUUUCUCGUUUUAUUUUUCAACGAUUUGGCGGAGAAGCUCCUCUUGUGAAUGGACUUUGGAUUUCUUGGAGCUGCGCUGCGGGUCCCACAGUGUGGCUUUCGGCCCGUGCUGUGCUGGCGCCUGCACUUCCUCUGGCGGGGCACGGGGUGGCGCUCCCUGGUAAAGCAGCGGCCAGGGGGAGCCGUGAGUGAGGCGCUGCCUCUCCCGCUGAAGCGGGUUCCAAGGCCACCGUGAGGGGGACCAUCCAUCCAGGAGAGUACUGGGCAGGCUGCAAAUGUCUGUGUUAAAACAGCUCUGCUGGGCUAAGACAGGACAGAAGCAGACAGCAGGUGGAUGAGACACAAUUUCCUAUCCAGCAGAACCUGCAGCAAGCUCCACAGCACCCUCCAUGGGCUCAGUCUUGCUCCCGGGAAGAUGGUUAAUUCCAUCAGCUCCUUCUGGCCGGCAGCAGGAAGAGUGGCCCUGUGUGUGCCAGGCCCUGCAGUCUCUCCUCUCAGCUGGUGUCUCCAGUGAGGGACCUGAGUCAUCGCACACAUGAGCCUGUGCUCAGCCUGCACAUCUCCCGCCUCCCACCAGCUGCUCCUCAACUGCCAGGGCCAGACUGUGGCAAAAUCUCACUCCUCUGCCGAUGCUGGGGUUUCCCUCGUGUCUGGGAGGUGGUGUGCUUGGUGGCCUGAGCACUGCAGUGAAUCCAUGUUUCCCUCCCAGCACCCUGUUCUGUCCUCCAACUUGGCCGACAGCUCUGGCCAGGGACGCAGCCCAGCUGGUGCCCACCCCGCACUCUGUCCAUUUCAUAAGAGCCCUUGGUUUCCUCACUUCCCUCAGAUUUUGCCAAGAGAAUGGUCCUGGUGUGGCCCAGAAAGGCCAGCGGGGUGCAGCCUGGGACUGAAAGCAGAGGCGGCUCUGGUGGGGAAAAAGUAGCUCUCCCAGCCUAGCCCUACUGGUGGGCGGCACCUCCUGGCUCCAGGCCAUCUUUUGUCCCAGUCCUAGGUAAGAAAAACACAAACAAAAGCCAGUCCCAUGGCACUCGAGAAGCAGGAGGCCGUUCCCUGACAGCAACAUGCUGUGUGCACAGACACACGGGUGGACAGGAGGCAGAGCUCGGGGUUGCUGCGGAGCGGGCAGGACACUGGAGCGGCAGGCAGUGCGGACCCGCCGGGCAGCCGUGCACGGUUGUCGUCCUCAGCGGCAGGAGCCAGUUUGUUGCUCAGGGCCUUGUCUUUUUACAAAGAGCCCCAGGCCCCGGGGGCUUCUCUGGGUGCCUCUUUGCUGCCAUGUCUGCACGCGGGCGGAGAGCAGACCAGGCUACCGACCCUCUCGCUUUGCUGUCUUCACGUGGAAAAGCCAGUGUCGUAGCCCCAAAGGAGGGGAAACUGUAUUGAUUUGGGGAGCCUCUAUGUUGAUUUCAAAACAGAUUGUCUCCUGUGUUCUCAAAGACUGGAAGCGAACCCCACAACCGCCUUAGGCCACAAAAGCUUUAUCCUUUCUAAUUAGCAUCCCUGUGACCUGCUCUGCGCCCUGCAGAUAUUUUGCUCAGCCAGCCAGAAGGAGGGAGGCCAGACACCAGCCCCCACAGACCUGCGGCUGCGACCCCCUGCCUGGGGACGAUGGGGUCGGGGUCCAGUAGCUGCCCCAGAAACAAGUGGGGCUGCAGGAGGCUGAUGGUGAGCUUGGAGGUUGGCAGAAUUCUAAAUCUGGGCACUGCAGGGUCCCCACAGGUCACGACCCUACUCUGCUCCACCCAGGCUCCGGAGGACCUGAGCAGGAACCUCUGCAGGGGGGGCCCGGGGCUCCCUGUCCUCUCAGCAGCCGGCAGUGCUCCCUGACAGCCCGGGCCUCUCCCUCCAGUAGUUCGGUAGUUUGCUGUCACCAACAUGGCUGGGCCUGGGACAGGCUCCUCCUCUCCCUCCAGAAGCCAGGCAGUCCCUCCUGCCUCAGUUUCUCAGACUAGGCCGCCUCUCCCAUCGCGAGACACUGAAGACCCUCAGCUGUUUCCAUCUGCCCAGUCUGACUGCUGGAUCGCCCUCUGUGUGCGUUGGUUUGCUGUGUUCUUGCUACUCGCCCUUGGAUAAGAUUUCUUCUCUACUCAUGAAGCUGCGUGUCCUGGAGGGCAGGGCCGCACCUCACAUGCAUGUUGCCCACAUAGCUCAGCAACAGAUGCUCUCACGCUUGUUAAAAGUAAAACCGGGCCAGGCGCAGUGGCUCACGCCUGUAAUCCCAGCACUUUGGGAGGCCGAGGUGGGUGGAUCACCUGAAGUCAGGAGUUUGAGACUAGCCUGACCAACAUGGAGAAAUCCCGUCUCUACUAAAAAUACAAAAAAUUAGCUGGGCGUGGUGGCACAUGCCUGUAAUCCCAGCUACUCGGAGGCAGGAGAAUUGCUUGAACCCAGGAGGCGGAGGUUGCGGUGAGCCAAGAUCACGCCAUAGCAAUUGCACUCCGGCCUGGGCAACAAGAGCAAAACUCUGUCAAAAAG</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2566</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>URS000075BB37</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>UGUCCUCCAUUGUAAGAUAAAAAGAGCUACCUAAGAGAUCUGUGGCUCAGUUCCUUUUGUUCAGUAUAUAUACCUCAGGGUAAAGGACCUAAGGCUCUGGCACUUCCUACAUAAUUUGUUCAUAAAAAUAAUUUUCUGUACCUGUAGGUGCAGGGAUUCAUAGUGAUUUUUCUGUUUUAAAAAAUAUCUUUCUACACUGUCUGAUUUUUAAAAAUGAGAUUAUCAGUAUAAAAGAAAUACAGCUAUUUUGUAAAAGAAAAAUACAGGAGAAAAAGGAUAAAGCUACUUUGUUUUAAAACGCAGUAUCAUUAAAACAAAAACAAACCAAAUUUGUUCUAAGUUUGACUUUAGAGUCAGGAAACUUAAGCUUACAUUUUUGGUCUGCCAUCUAUUACUUUUAAAGCUUGGGCAAAUUAUUCAUUUGAAGUCUAAAUUUAUUAAUCUGUUAAUGGGAACAGAUUAGAAAUCUUCAGAGAAGCUCUAGCCUUUGUAACAUUGUGACUAUAAUGCUGAGAACUGCUUCACUCAUCCCAUUCAUAUUUUAAAAAUACUAAUAUUUUGUGUUUGAGCAUUUUAAUAGGCUCAGAAACUUAAAAAUGAUGUUUCUUUUCUAACAACAUACUCUUUUCAAUGGGAUAUUAUGGUUGUUAUUAUUUAACAUGACAUUUAGGGACUCAACAUACAUUAAGGUGAUGGCACUAAGAUAAAUGUAGAAAUAACCAGUACCAUGUAAUUUUCAUAAGUGCUUAAAUUGUUGGUAAACAAUUUUAUGAGUUGGAGGUGUUGAAGCAAAUAUUAUUAAUAUUUGAACAUAAAAGCUGAUCAAAGGGGCCUGGUCCACAGAAGAUGUUUAUUUGAUGUAACAAAACAAUACAGUUAGUGUUAGAUCCAACCACAAAGAGCAAAAGGAAUGAAAAAUUUGUACAAUGUACAUAGAAAAAACAAGAUAUUUACUGUGACAACUAUAUAUUCCUAAAAUAAUGCUUCUAAAAUUACUCAAUUAUUGAAAUCUACAUGAAAAAAAGGAUGUUAAUAGCGACAAAGUGCAUAAAAUCAAACAUUGUAUUUUGAGCAAAUUAACAUACUAGGCAAUUUUGCUAAGAAUGCAUGAUUUUUUUUUUCUUGUUUACAGUCUGCUCAAAAUAUCUUUAUACCAACAGGGUAGGCAGAACAUUUAGGUUUAAUAUCAGUUACACAAUAUUAGCAUAAACUUCCACAACUACAUAGGGUAUUGUUUUCUUUUGAGCUGGCAAAGUGACUAUAGAAACAUCAGAUGAUUUCUCUGAAUUGAGAAUUUUAUCCAAAUAAAUGCCACAUACCUUCUAGAUAUAUGCAUAUCUUUCUAUAUUAUGUAAAUGGCUUUACCCAUUUAAAUAAUAAACCAUACAGCAUUUAAGAAUCAUUAUUAUAUGAUUAACAAUGUCAUGUUCCAGGUUUAACAAUUUCAUAGGCCAAAAAAAAUUUCUUCUUAAAAACUAGUUUUAUAAACGCAGAAUAUAUUCCAUGAGUAACUGCUGGUAUUUUUUAAGAAAAUAUAUUGUGCAAUUGUGGCUACCACGUACUGCUGGCAAAGCAUUAUUAUUUAUGUAAAAUGUGAAAAAAAAGGUGUAAAAAUUUUUCAACUGCCUAUGAUCAUGAUGAAAGGUUACUGCCUUCUUACAAAAAUUAUAUUGGCAUCUUCUUAAAAAUAAUUCGAAAAAGGGAUAAACUCCCUAGCCAAAAAUAAAUAAAUAAAAAGGUGCAUUUUUUAAAAUGAUGCUACUGCAAUGCAAUGGUUUAAAUACCAAAAAACUGAGAAAAUGAGCUGUCUGUGAUCCAGCAUUAAAGAACAUACUAAAAAAGAGCAUUAAUGUAAAUUAAGUAGAAAGGGGAUCAAAAUUGAACUAACCAAGUUUGUGCAGUAUUGUAGCCAGGCUUCUAAAAUUAGAUGUAGAAAAUAUAAAUAGACUGCUUUAGGUAAUGAGCCACCAGUGUCCAAAAAAAGGAAUGAAAUUAAGAAAAAGCUCAGUUAACUUGAUCCAAAGCUCUGAGUAAUUCUUCACCCUGCAGUA</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>2051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>